<commit_message>
pushes since a lot of time
</commit_message>
<xml_diff>
--- a/analyse_M2/data/donneesAgency.xlsx
+++ b/analyse_M2/data/donneesAgency.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\l2export\iss02.cenir\analyse\meeg\BETAPARK\code\PYTHON_SCRIPTS\M2data_analysis\analyse_M2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C157BECB-6C0C-450C-8F62-1906248904AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2606F12C-7796-4026-A8B3-3F7908201D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="182">
   <si>
     <t>num_sujet</t>
   </si>
@@ -368,6 +368,219 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>logPendule_12-15</t>
+  </si>
+  <si>
+    <t>logMain_12-15</t>
+  </si>
+  <si>
+    <t>-0.21098646992113684</t>
+  </si>
+  <si>
+    <t>-0.10950290292094512</t>
+  </si>
+  <si>
+    <t>-0.3045938494876628</t>
+  </si>
+  <si>
+    <t>0.023811341069590326</t>
+  </si>
+  <si>
+    <t>0.027344537143775764</t>
+  </si>
+  <si>
+    <t>-0.19347242174437226</t>
+  </si>
+  <si>
+    <t>-0.28783401929208363</t>
+  </si>
+  <si>
+    <t>-0.1779380425896484</t>
+  </si>
+  <si>
+    <t>-0.27306439600317445</t>
+  </si>
+  <si>
+    <t>-0.20381686144500985</t>
+  </si>
+  <si>
+    <t>-0.1639899577034517</t>
+  </si>
+  <si>
+    <t>-0.24097174412414651</t>
+  </si>
+  <si>
+    <t>-0.26888876961221925</t>
+  </si>
+  <si>
+    <t>-0.13434131029707796</t>
+  </si>
+  <si>
+    <t>-0.14414823136409075</t>
+  </si>
+  <si>
+    <t>0.05767838680199748</t>
+  </si>
+  <si>
+    <t>-0.17930659394766216</t>
+  </si>
+  <si>
+    <t>-0.1560230169853511</t>
+  </si>
+  <si>
+    <t>-0.21991180581882955</t>
+  </si>
+  <si>
+    <t>-0.30897672725920944</t>
+  </si>
+  <si>
+    <t>-0.5823658177366355</t>
+  </si>
+  <si>
+    <t>-0.545637074888903</t>
+  </si>
+  <si>
+    <t>-0.34883226293254177</t>
+  </si>
+  <si>
+    <t>-0.23595105074960743</t>
+  </si>
+  <si>
+    <t>-0.11843638498745385</t>
+  </si>
+  <si>
+    <t>-0.34045230120266257</t>
+  </si>
+  <si>
+    <t>-0.08488640871207545</t>
+  </si>
+  <si>
+    <t>-0.26627763530558246</t>
+  </si>
+  <si>
+    <t>-0.2718337538989065</t>
+  </si>
+  <si>
+    <t>-0.3842998826109755</t>
+  </si>
+  <si>
+    <t>-0.13550840819437404</t>
+  </si>
+  <si>
+    <t>-0.23036143578881754</t>
+  </si>
+  <si>
+    <t>-0.3175655152104123</t>
+  </si>
+  <si>
+    <t>-0.1793131226119734</t>
+  </si>
+  <si>
+    <t>-0.29422015438441607</t>
+  </si>
+  <si>
+    <t>-0.5580948452892113</t>
+  </si>
+  <si>
+    <t>-0.38351693177256707</t>
+  </si>
+  <si>
+    <t>-0.2872697942553085</t>
+  </si>
+  <si>
+    <t>-0.2881739642465899</t>
+  </si>
+  <si>
+    <t>-0.35403283224346505</t>
+  </si>
+  <si>
+    <t>-0.16824965885472615</t>
+  </si>
+  <si>
+    <t>-0.2241509795155312</t>
+  </si>
+  <si>
+    <t>-0.2796042437299411</t>
+  </si>
+  <si>
+    <t>-0.6452905561102045</t>
+  </si>
+  <si>
+    <t>-0.44847424862170965</t>
+  </si>
+  <si>
+    <t>-0.2768411301864159</t>
+  </si>
+  <si>
+    <t>-0.06033701318122429</t>
+  </si>
+  <si>
+    <t>-0.4067259201581045</t>
+  </si>
+  <si>
+    <t>-0.06360797258274675</t>
+  </si>
+  <si>
+    <t>-0.07378478705718165</t>
+  </si>
+  <si>
+    <t>-0.3982227875356943</t>
+  </si>
+  <si>
+    <t>-0.3309579898867294</t>
+  </si>
+  <si>
+    <t>-0.3050488645161073</t>
+  </si>
+  <si>
+    <t>-0.5152210840569853</t>
+  </si>
+  <si>
+    <t>-0.2487752420670996</t>
+  </si>
+  <si>
+    <t>-0.05717998147738178</t>
+  </si>
+  <si>
+    <t>-0.23168480434734134</t>
+  </si>
+  <si>
+    <t>-0.47457578394215805</t>
+  </si>
+  <si>
+    <t>-0.20171218134529745</t>
+  </si>
+  <si>
+    <t>-0.30250502318091455</t>
+  </si>
+  <si>
+    <t>0.07210179907117972</t>
+  </si>
+  <si>
+    <t>-0.13376613894353825</t>
+  </si>
+  <si>
+    <t>-0.05455529683888913</t>
+  </si>
+  <si>
+    <t>-0.047102871333833216</t>
+  </si>
+  <si>
+    <t>-0.30669972184476957</t>
+  </si>
+  <si>
+    <t>-0.6581828718816704</t>
+  </si>
+  <si>
+    <t>-0.3618193750874174</t>
+  </si>
+  <si>
+    <t>-0.3378361477272832</t>
+  </si>
+  <si>
+    <t>logMainIllusion_12-15</t>
   </si>
 </sst>
 </file>
@@ -852,9 +1065,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CU1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="CV1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="DD24" sqref="DD24"/>
+      <selection pane="bottomLeft" activeCell="DH2" sqref="DH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -862,7 +1075,7 @@
     <col min="1" max="1025" width="14.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:109" s="4" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:112" s="4" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1190,8 +1403,17 @@
       <c r="DE1" s="2" t="s">
         <v>108</v>
       </c>
+      <c r="DF1" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="DG1" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="DH1" s="4" t="s">
+        <v>181</v>
+      </c>
     </row>
-    <row r="2" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -1526,8 +1748,17 @@
         <f t="shared" ref="DE2:DE24" si="4">LOG10(AU2)</f>
         <v>-5.3875380799243075E-2</v>
       </c>
+      <c r="DF2" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="DG2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="DH2" s="1">
+        <v>-0.27204405790817499</v>
+      </c>
     </row>
-    <row r="3" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1862,8 +2093,17 @@
         <f t="shared" si="4"/>
         <v>0.28296599569523856</v>
       </c>
+      <c r="DF3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="DG3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="DH3" s="1" t="s">
+        <v>159</v>
+      </c>
     </row>
-    <row r="4" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -2198,8 +2438,17 @@
         <f t="shared" si="4"/>
         <v>-9.4871068023808916E-2</v>
       </c>
+      <c r="DF4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="DG4" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="DH4" s="1" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="5" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>5</v>
       </c>
@@ -2534,8 +2783,17 @@
         <f t="shared" si="4"/>
         <v>-0.23601078152772695</v>
       </c>
+      <c r="DF5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="DG5" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="DH5" s="1" t="s">
+        <v>161</v>
+      </c>
     </row>
-    <row r="6" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>6</v>
       </c>
@@ -2870,8 +3128,17 @@
         <f t="shared" si="4"/>
         <v>4.397945280400789E-2</v>
       </c>
+      <c r="DF6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="DG6" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="DH6" s="1" t="s">
+        <v>162</v>
+      </c>
     </row>
-    <row r="7" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>7</v>
       </c>
@@ -3206,8 +3473,17 @@
         <f t="shared" si="4"/>
         <v>0.10551018476997394</v>
       </c>
+      <c r="DF7" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="DG7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="DH7" s="1" t="s">
+        <v>163</v>
+      </c>
     </row>
-    <row r="8" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>8</v>
       </c>
@@ -3542,8 +3818,17 @@
         <f t="shared" si="4"/>
         <v>-2.9842064363711878E-2</v>
       </c>
+      <c r="DF8" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="DG8" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="DH8" s="1" t="s">
+        <v>164</v>
+      </c>
     </row>
-    <row r="9" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>9</v>
       </c>
@@ -3878,8 +4163,17 @@
         <f t="shared" si="4"/>
         <v>0.47278081986520942</v>
       </c>
+      <c r="DF9" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="DG9" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="DH9" s="1" t="s">
+        <v>165</v>
+      </c>
     </row>
-    <row r="10" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>10</v>
       </c>
@@ -4214,8 +4508,17 @@
         <f t="shared" si="4"/>
         <v>-6.3989204284790407E-2</v>
       </c>
+      <c r="DF10" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="DG10" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="DH10" s="1" t="s">
+        <v>166</v>
+      </c>
     </row>
-    <row r="11" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>11</v>
       </c>
@@ -4550,8 +4853,17 @@
         <f t="shared" si="4"/>
         <v>0.62077023967108891</v>
       </c>
+      <c r="DF11" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="DG11" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="DH11" s="1" t="s">
+        <v>167</v>
+      </c>
     </row>
-    <row r="12" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>12</v>
       </c>
@@ -4886,8 +5198,17 @@
         <f t="shared" si="4"/>
         <v>3.6487989851363353E-2</v>
       </c>
+      <c r="DF12" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DG12" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="DH12" s="1" t="s">
+        <v>168</v>
+      </c>
     </row>
-    <row r="13" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>13</v>
       </c>
@@ -5222,8 +5543,17 @@
         <f t="shared" si="4"/>
         <v>8.8179321361998755E-2</v>
       </c>
+      <c r="DF13" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DG13" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="DH13" s="1" t="s">
+        <v>169</v>
+      </c>
     </row>
-    <row r="14" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>14</v>
       </c>
@@ -5558,8 +5888,17 @@
         <f t="shared" si="4"/>
         <v>1.7867718963505686E-2</v>
       </c>
+      <c r="DF14" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="DG14" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="DH14" s="1" t="s">
+        <v>170</v>
+      </c>
     </row>
-    <row r="15" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>15</v>
       </c>
@@ -5894,8 +6233,17 @@
         <f t="shared" si="4"/>
         <v>0.18975820366889395</v>
       </c>
+      <c r="DF15" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="DG15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="DH15" s="1" t="s">
+        <v>171</v>
+      </c>
     </row>
-    <row r="16" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>16</v>
       </c>
@@ -6230,8 +6578,17 @@
         <f t="shared" si="4"/>
         <v>-6.2147906732140823E-2</v>
       </c>
+      <c r="DF16" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="DG16" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="DH16" s="1" t="s">
+        <v>172</v>
+      </c>
     </row>
-    <row r="17" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>17</v>
       </c>
@@ -6566,8 +6923,17 @@
         <f t="shared" si="4"/>
         <v>8.2066934285113011E-2</v>
       </c>
+      <c r="DF17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="DG17" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="DH17" s="1" t="s">
+        <v>173</v>
+      </c>
     </row>
-    <row r="18" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>18</v>
       </c>
@@ -6902,8 +7268,17 @@
         <f t="shared" si="4"/>
         <v>0.25425052601579778</v>
       </c>
+      <c r="DF18" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="DG18" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="DH18" s="1" t="s">
+        <v>174</v>
+      </c>
     </row>
-    <row r="19" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>19</v>
       </c>
@@ -7238,8 +7613,17 @@
         <f t="shared" si="4"/>
         <v>-5.1381158678629697E-2</v>
       </c>
+      <c r="DF19" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="DG19" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="DH19" s="1" t="s">
+        <v>175</v>
+      </c>
     </row>
-    <row r="20" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>20</v>
       </c>
@@ -7574,8 +7958,17 @@
         <f t="shared" si="4"/>
         <v>-8.0153108571170417E-2</v>
       </c>
+      <c r="DF20" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="DG20" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="DH20" s="1" t="s">
+        <v>176</v>
+      </c>
     </row>
-    <row r="21" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>21</v>
       </c>
@@ -7910,8 +8303,17 @@
         <f t="shared" si="4"/>
         <v>-0.1398492296819186</v>
       </c>
+      <c r="DF21" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="DG21" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="DH21" s="1" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="22" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>22</v>
       </c>
@@ -8246,8 +8648,17 @@
         <f t="shared" si="4"/>
         <v>-0.12152075945781179</v>
       </c>
+      <c r="DF22" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="DG22" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="DH22" s="1" t="s">
+        <v>178</v>
+      </c>
     </row>
-    <row r="23" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>23</v>
       </c>
@@ -8582,8 +8993,17 @@
         <f t="shared" si="4"/>
         <v>-0.13872702109393326</v>
       </c>
+      <c r="DF23" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="DG23" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="DH23" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
-    <row r="24" spans="1:109" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:112" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>24</v>
       </c>
@@ -8926,33 +9346,42 @@
         <f t="shared" si="4"/>
         <v>-0.25052134951230504</v>
       </c>
+      <c r="DF24" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="DG24" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="DH24" s="1" t="s">
+        <v>180</v>
+      </c>
     </row>
-    <row r="27" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
     </row>
-    <row r="28" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
     </row>
-    <row r="29" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
     </row>
-    <row r="30" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
     </row>
-    <row r="31" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
     </row>
-    <row r="32" spans="1:109" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>

</xml_diff>